<commit_message>
Phase 3.9-3.15: FHIR validation error reduction
Error progression:
- Phase 3.9:  72 errors (baseline)
- Phase 3.12: 70 errors (-2)
- Phase 3.13: 38 errors (-32, -45.7%)
- Phase 3.14: 30 errors (-8, -21.1%)
- Phase 3.15: 31 errors (+1)

Total reduction: 72 → 31 errors (-56.9%)

Key fixes:
- Invalid LOINC/SNOMED codes replaced with local codes
- ValueSet binding corrections
- R5 extension compatibility fixes
- CodeableConcept conflict resolutions

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/CodeSystem-lifestyle-observation-cs.xlsx
+++ b/output/CodeSystem-lifestyle-observation-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="194">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-01T16:36:18+01:00</t>
+    <t>2025-10-01T23:24:47+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -138,7 +138,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>42</t>
+    <t>49</t>
   </si>
   <si>
     <t>Level</t>
@@ -453,6 +453,15 @@
     <t>Comprehensive balance and stability assessment</t>
   </si>
   <si>
+    <t>balance-status</t>
+  </si>
+  <si>
+    <t>Balance status</t>
+  </si>
+  <si>
+    <t>Qualitative status of balance (normal, impaired, etc.)</t>
+  </si>
+  <si>
     <t>gait-assessment</t>
   </si>
   <si>
@@ -525,6 +534,24 @@
     <t>Status of ovulation as measured by consumer fertility tracking device</t>
   </si>
   <si>
+    <t>sleep-monitoring-device</t>
+  </si>
+  <si>
+    <t>Sleep monitoring device</t>
+  </si>
+  <si>
+    <t>Device for monitoring and tracking sleep patterns and sleep quality metrics</t>
+  </si>
+  <si>
+    <t>environmental-sensor</t>
+  </si>
+  <si>
+    <t>Environmental sensor device</t>
+  </si>
+  <si>
+    <t>Device for monitoring environmental conditions such as noise, temperature, humidity, and UV exposure</t>
+  </si>
+  <si>
     <t>body-composition-panel</t>
   </si>
   <si>
@@ -532,6 +559,42 @@
   </si>
   <si>
     <t>Panel for comprehensive body composition measurements from bioimpedance analysis</t>
+  </si>
+  <si>
+    <t>mindfulness-session</t>
+  </si>
+  <si>
+    <t>Mindfulness practice session</t>
+  </si>
+  <si>
+    <t>A session of mindfulness meditation or practice including breathing exercises, body scans, or mindful awareness</t>
+  </si>
+  <si>
+    <t>relaxation-response</t>
+  </si>
+  <si>
+    <t>Relaxation response observation</t>
+  </si>
+  <si>
+    <t>Subjective observation of the relaxation response experienced during or after mindfulness or relaxation practice</t>
+  </si>
+  <si>
+    <t>mindfulness-type</t>
+  </si>
+  <si>
+    <t>Type of mindfulness practice</t>
+  </si>
+  <si>
+    <t>The specific type or technique of mindfulness or meditation practice performed</t>
+  </si>
+  <si>
+    <t>water-intake</t>
+  </si>
+  <si>
+    <t>Water intake volume</t>
+  </si>
+  <si>
+    <t>Daily water consumption measured in liters or milliliters</t>
   </si>
 </sst>
 </file>
@@ -884,7 +947,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1492,6 +1555,104 @@
         <v>172</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="D44" t="s" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="D46" t="s" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="D47" t="s" s="2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="D48" t="s" s="2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="D49" t="s" s="2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="D50" t="s" s="2">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: Add inflammatory_markers.md - Task 2.2.8 complete
Completes Inflammatory Markers documentation (8/8 tasks):
- Clinical background and evidence (Williams 2019, Pearson 2003, Ridker 2002)
- Profile descriptions (CRP, hs-CRP, IL-6, TNF-α, Correlation)
- hs-CRP cardiovascular risk classification (AHA/CDC guidelines)
- ValueSets: InflammatoryMarkerVS, HsCRPRiskCategoryVS, HRVInflammationTrendVS
- Usage examples with JSON
- Clinical integration workflow
- Learning Health System integration

SUSHI: 0 errors, 0 warnings

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/CodeSystem-lifestyle-observation-cs.xlsx
+++ b/output/CodeSystem-lifestyle-observation-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="233">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-03T16:37:46+01:00</t>
+    <t>2025-11-27T11:57:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -138,7 +138,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>54</t>
+    <t>62</t>
   </si>
   <si>
     <t>Level</t>
@@ -640,6 +640,78 @@
   </si>
   <si>
     <t>Measurement of heart rate variability (HRV)</t>
+  </si>
+  <si>
+    <t>alcohol-type</t>
+  </si>
+  <si>
+    <t>Type of alcoholic beverage</t>
+  </si>
+  <si>
+    <t>Type of alcoholic beverage consumed (beer, wine, spirits, etc.)</t>
+  </si>
+  <si>
+    <t>caffeine-source</t>
+  </si>
+  <si>
+    <t>Caffeine source</t>
+  </si>
+  <si>
+    <t>Source of dietary caffeine intake (coffee, tea, energy drinks, etc.)</t>
+  </si>
+  <si>
+    <t>last-caffeine-time</t>
+  </si>
+  <si>
+    <t>Time of last caffeine intake</t>
+  </si>
+  <si>
+    <t>Date and time of the most recent caffeine consumption</t>
+  </si>
+  <si>
+    <t>substance-frequency</t>
+  </si>
+  <si>
+    <t>Frequency of substance use</t>
+  </si>
+  <si>
+    <t>How often a substance is used (daily, weekly, monthly, etc.)</t>
+  </si>
+  <si>
+    <t>last-use-date</t>
+  </si>
+  <si>
+    <t>Date of last substance use</t>
+  </si>
+  <si>
+    <t>Date when a substance was last used</t>
+  </si>
+  <si>
+    <t>substance-use-summary</t>
+  </si>
+  <si>
+    <t>Substance use summary</t>
+  </si>
+  <si>
+    <t>Comprehensive summary of all substance use patterns for lifestyle medicine assessment</t>
+  </si>
+  <si>
+    <t>substance-risk-level</t>
+  </si>
+  <si>
+    <t>Overall substance use risk level</t>
+  </si>
+  <si>
+    <t>Aggregate risk assessment based on all substance use patterns</t>
+  </si>
+  <si>
+    <t>hrv-inflammation-correlation</t>
+  </si>
+  <si>
+    <t>HRV-Inflammation correlation assessment</t>
+  </si>
+  <si>
+    <t>Assessment of the correlation between heart rate variability metrics (especially RMSSD) and inflammatory biomarkers (CRP, IL-6). Based on RS1 systematic review finding: inverse correlation between vagal tone and systemic inflammation via cholinergic anti-inflammatory pathway (Tracey 2002).</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1768,6 +1840,118 @@
         <v>208</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="D56" t="s" s="2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="D57" t="s" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="D58" t="s" s="2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="D59" t="s" s="2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="C60" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="D60" t="s" s="2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="C61" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="D61" t="s" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="C62" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="D62" t="s" s="2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C63" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="D63" t="s" s="2">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>